<commit_message>
updated preliminary package loading roster for each truck fixed hash added notes section to csv added notes field to Package class added Truck and Driver classes
</commit_message>
<xml_diff>
--- a/loaded_trucks.xlsx
+++ b/loaded_trucks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwils\PycharmProjects\notUPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwils\iCloudDrive\Documents\WGU\notUPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7746495-F228-4EF7-857D-F2A29AF2587D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D746CB73-72BE-43C9-B81B-51DE0C273C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9090" yWindow="795" windowWidth="19560" windowHeight="16695" xr2:uid="{BC7694C7-DF4C-403A-ACEF-7D229F10FCCD}"/>
+    <workbookView xWindow="15720" yWindow="5220" windowWidth="24045" windowHeight="15345" xr2:uid="{BC7694C7-DF4C-403A-ACEF-7D229F10FCCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Truck 1" sheetId="2" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,11 +720,11 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
@@ -732,21 +732,21 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>84104</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
+        <v>84115</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -755,21 +755,21 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>84104</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
+        <v>84115</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G10">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -778,21 +778,21 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>84115</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.4375</v>
+        <v>84106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -801,21 +801,21 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>84106</v>
+        <v>84104</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -824,13 +824,13 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>84115</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.4375</v>
+        <v>84104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -840,10 +840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19155DCA-40E5-4238-B48E-D9002D08A78F}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,33 +1096,36 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>84118</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
+        <v>84119</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1131,21 +1134,21 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>84118</v>
+        <v>84103</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1154,21 +1157,24 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>84105</v>
+        <v>84119</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1177,13 +1183,62 @@
         <v>2</v>
       </c>
       <c r="E14">
-        <v>84103</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3</v>
+        <v>84119</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>84117</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>84117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1193,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB2CBEC-B5B5-4E45-98BE-BA4D7FAE8412}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,36 +1261,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1">
-        <v>84119</v>
-      </c>
-      <c r="F1" s="1">
-        <v>0.4375</v>
+        <v>84103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
       </c>
       <c r="G1">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1244,24 +1299,21 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>84103</v>
+        <v>84118</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1270,24 +1322,21 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>84117</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.4375</v>
+        <v>84105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -1296,21 +1345,24 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>84117</v>
+        <v>84115</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1319,82 +1371,76 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>84115</v>
+        <v>84118</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6">
-        <v>84119</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.4375</v>
+        <v>84121</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
       <c r="E7">
-        <v>84119</v>
+        <v>84107</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
       </c>
       <c r="E8">
-        <v>84121</v>
+        <v>84119</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
@@ -1405,33 +1451,33 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
       </c>
       <c r="E9">
-        <v>84107</v>
+        <v>84115</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1440,21 +1486,21 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>84119</v>
+        <v>84106</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1469,52 +1515,6 @@
         <v>3</v>
       </c>
       <c r="G11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>84106</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>84115</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
loaded packages onto trucks deleted extra rows from distance.csv
</commit_message>
<xml_diff>
--- a/loaded_trucks.xlsx
+++ b/loaded_trucks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwils\iCloudDrive\Documents\WGU\notUPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwils\PycharmProjects\notUPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D746CB73-72BE-43C9-B81B-51DE0C273C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69BF7E9-7748-457E-B926-01B4B7024253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="5220" windowWidth="24045" windowHeight="15345" xr2:uid="{BC7694C7-DF4C-403A-ACEF-7D229F10FCCD}"/>
+    <workbookView xWindow="26790" yWindow="5190" windowWidth="24045" windowHeight="15345" activeTab="2" xr2:uid="{BC7694C7-DF4C-403A-ACEF-7D229F10FCCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Truck 1" sheetId="2" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E73AF12-1365-4D45-AA08-5BC64ADE49B4}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,86 +526,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2">
-        <v>84104</v>
-      </c>
-      <c r="F1" s="3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>84115</v>
+      </c>
+      <c r="F1" s="1">
         <v>0.4375</v>
       </c>
-      <c r="G1" s="2">
-        <v>2</v>
-      </c>
+      <c r="G1">
+        <v>21</v>
+      </c>
+      <c r="H1"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>84117</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="G2" s="2">
-        <v>88</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>84106</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>44</v>
+      </c>
+      <c r="H2"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2">
-        <v>84117</v>
+        <v>84104</v>
       </c>
       <c r="F3" s="3">
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="G3" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -620,110 +619,114 @@
         <v>88</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>84115</v>
+        <v>84117</v>
       </c>
       <c r="F5" s="3">
-        <v>0.4375</v>
+        <v>0.375</v>
       </c>
       <c r="G5" s="2">
-        <v>37</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>84117</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="G6" s="2">
+        <v>88</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
         <v>84115</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>84104</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>9</v>
+      <c r="F7" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="G7" s="2">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>84117</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.4375</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
+      <c r="A8" s="2">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>84115</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -732,44 +735,44 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>84115</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.4375</v>
+        <v>84104</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>84115</v>
+        <v>84117</v>
       </c>
       <c r="F10" s="1">
         <v>0.4375</v>
       </c>
       <c r="G10">
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -778,21 +781,21 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>84106</v>
+        <v>84104</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
       </c>
       <c r="G11">
-        <v>44</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -807,15 +810,15 @@
         <v>3</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -824,16 +827,19 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>84104</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
+        <v>84115</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G13">
-        <v>88</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H13">
+    <sortCondition ref="A1:A13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -843,7 +849,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,36 +886,33 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>84111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>84123</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -920,22 +923,22 @@
       <c r="E3">
         <v>84119</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
+      <c r="F3" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G3">
         <v>88</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -944,24 +947,21 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>84111</v>
+        <v>84106</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
       </c>
       <c r="G4">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -970,44 +970,44 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>84111</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.4375</v>
+        <v>84103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6">
-        <v>84111</v>
+        <v>84119</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -1016,44 +1016,50 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>84103</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.4375</v>
+        <v>84123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>84117</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>84106</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>8</v>
+      <c r="H8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -1062,70 +1068,67 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>84106</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.4375</v>
+        <v>84117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>84119</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
+        <v>84106</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>84119</v>
+        <v>84103</v>
       </c>
       <c r="F11" s="1">
         <v>0.4375</v>
       </c>
       <c r="G11">
-        <v>88</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1134,13 +1137,13 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>84103</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
+        <v>84119</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.4375</v>
       </c>
       <c r="G12">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1171,13 +1174,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -1185,19 +1188,22 @@
       <c r="E14">
         <v>84119</v>
       </c>
-      <c r="F14" s="1">
-        <v>0.4375</v>
+      <c r="F14" t="s">
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -1206,24 +1212,21 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>84117</v>
+        <v>84111</v>
       </c>
       <c r="F15" s="1">
         <v>0.4375</v>
       </c>
       <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -1232,16 +1235,22 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>84117</v>
+        <v>84111</v>
       </c>
       <c r="F16" t="s">
         <v>3</v>
       </c>
       <c r="G16">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1250,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB2CBEC-B5B5-4E45-98BE-BA4D7FAE8412}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,10 +1270,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1273,24 +1282,21 @@
         <v>2</v>
       </c>
       <c r="E1">
-        <v>84103</v>
+        <v>84115</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1299,13 +1305,16 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>84118</v>
+        <v>84103</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1333,10 +1342,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -1345,24 +1354,21 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>84115</v>
+        <v>84118</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
       </c>
       <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1371,44 +1377,44 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>84118</v>
+        <v>84119</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6">
-        <v>84121</v>
+        <v>84115</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
@@ -1417,21 +1423,21 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>84107</v>
+        <v>84121</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1440,44 +1446,44 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>84119</v>
+        <v>84118</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
       </c>
       <c r="E9">
-        <v>84115</v>
+        <v>84107</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1486,21 +1492,24 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>84106</v>
+        <v>84115</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1509,16 +1518,19 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>84115</v>
+        <v>84106</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
       </c>
       <c r="G11">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H11">
+    <sortCondition ref="A1:A11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>